<commit_message>
Updated data import file in materials
</commit_message>
<xml_diff>
--- a/materials/Session 1/Задание на работу.xlsx
+++ b/materials/Session 1/Задание на работу.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Championship2026Preparation\materials\Session 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B95461D-5F00-4DC4-9B7F-E0033A8E0A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A9DBC9-E74A-4F30-BA84-EC03ADE7FAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23596" windowHeight="15076" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,6 +38,7 @@
     <author>tc={14E9D2C1-16EA-4431-A2FB-810EA1F27F07}</author>
     <author>tc={CF93BBE7-D3C0-4EDF-8667-9CB44F7EA933}</author>
     <author>tc={6471FFFE-A0EB-4FB6-93DE-565267D3445F}</author>
+    <author>tc={F1401E3A-337D-4B6F-809D-DFDE3B1CA8A9}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5A1F287D-9AE4-4C87-8A99-D99615BD3EF1}">
@@ -128,12 +129,20 @@
     Плановые часы в GitLab (Число 3,1)</t>
       </text>
     </comment>
+    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{F1401E3A-337D-4B6F-809D-DFDE3B1CA8A9}">
+      <text>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    Первая строка в ТЧ Работы Задания на работу поле Комментарий Строка</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Номер задания</t>
   </si>
@@ -262,6 +271,51 @@
   </si>
   <si>
     <t>Номер проекта</t>
+  </si>
+  <si>
+    <t>Текст задания</t>
+  </si>
+  <si>
+    <t>Сходить помыть подмыхи</t>
+  </si>
+  <si>
+    <t>Сделать сальтуху и сдать практику</t>
+  </si>
+  <si>
+    <t>Сходить в туалет с котом и попугаем</t>
+  </si>
+  <si>
+    <t>Разработать сайт</t>
+  </si>
+  <si>
+    <t>Скупить все золотое яблоко</t>
+  </si>
+  <si>
+    <t>Научиться писать на 1С</t>
+  </si>
+  <si>
+    <t>Стать 1С</t>
+  </si>
+  <si>
+    <t>Жить и умереть 1С</t>
+  </si>
+  <si>
+    <t>Валидация:</t>
+  </si>
+  <si>
+    <t>Валидация даты</t>
+  </si>
+  <si>
+    <t>Валидация статусов</t>
+  </si>
+  <si>
+    <t>Валидация факта и плана часов</t>
+  </si>
+  <si>
+    <t>Обязательность текста задания</t>
+  </si>
+  <si>
+    <t>В случае отсутствия данных не присутствующих в этой таблице выводить информационное сообщение в поле с ошибкой что "Нужно создать что-то там"</t>
   </si>
 </sst>
 </file>
@@ -289,8 +343,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -319,11 +372,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -649,15 +705,18 @@
   <threadedComment ref="K1" dT="2025-09-26T06:31:54.33" personId="{11D9141A-2134-40AB-999F-93BE59A8D8B3}" id="{6471FFFE-A0EB-4FB6-93DE-565267D3445F}">
     <text>Плановые часы в GitLab (Число 3,1)</text>
   </threadedComment>
+  <threadedComment ref="L1" dT="2025-09-26T20:43:36.53" personId="{11D9141A-2134-40AB-999F-93BE59A8D8B3}" id="{F1401E3A-337D-4B6F-809D-DFDE3B1CA8A9}">
+    <text>Первая строка в ТЧ Работы Задания на работу поле Комментарий Строка</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -672,9 +731,10 @@
     <col min="9" max="9" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.06640625" customWidth="1"/>
+    <col min="12" max="12" width="33.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -708,8 +768,11 @@
       <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -743,8 +806,11 @@
       <c r="K2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -778,8 +844,11 @@
       <c r="K3">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -813,8 +882,11 @@
       <c r="K4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -848,8 +920,11 @@
       <c r="K5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -883,8 +958,11 @@
       <c r="K6">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -918,8 +996,11 @@
       <c r="K7">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -953,8 +1034,11 @@
       <c r="K8">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -988,38 +1072,76 @@
       <c r="K9">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E13:G17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>